<commit_message>
New build of website after updating main
</commit_message>
<xml_diff>
--- a/StructureDefinition-cbs-co-condition.xlsx
+++ b/StructureDefinition-cbs-co-condition.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="308">
   <si>
     <t>Path</t>
   </si>
@@ -155,7 +155,7 @@
     <t>Detailed information about conditions, problems or diagnoses</t>
   </si>
   <si>
-    <t>The Case Based Surveillance Patient Profile is loosely based upon the US Core Patient Profile, which is in turn based on the core FHIR Patient Resource. It is designed to meet the needs of US public health case based surveillance while maintaining as much alignment with US Core profiles as possible.</t>
+    <t>A clinical condition, problem, diagnosis, or other event, situation, issue, or clinical concept that has risen to a level of concern.</t>
   </si>
   <si>
     <t>con-3:Condition.clinicalStatus SHALL be present if verificationStatus is not entered-in-error and category is problem-list-item {clinicalStatus.exists() or verificationStatus.coding.where(system='http://terminology.hl7.org/CodeSystem/condition-ver-status' and code = 'entered-in-error').exists() or category.select($this='problem-list-item').empty()}
@@ -544,6 +544,14 @@
   </si>
   <si>
     <t>0..1 to account for primarily narrative only resources.</t>
+  </si>
+  <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://loinc.org"/&gt;
+    &lt;code value="91558-7"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
     <t>example</t>
@@ -616,7 +624,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Patient|Group)
+    <t xml:space="preserve">Reference(http://cbsig.chai.gatech.edu/StructureDefinition/cbs-patient)
 </t>
   </si>
   <si>
@@ -954,7 +962,7 @@
     <t>Condition.evidence.detail</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Resource)
+    <t xml:space="preserve">Reference(http://cbsig.chai.gatech.edu/StructureDefinition/cbs-condition)
 </t>
   </si>
   <si>
@@ -2992,7 +3000,7 @@
         <v>42</v>
       </c>
       <c r="R16" t="s" s="2">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="S16" t="s" s="2">
         <v>42</v>
@@ -3007,13 +3015,13 @@
         <v>42</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>42</v>
@@ -3046,27 +3054,27 @@
         <v>65</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3092,13 +3100,13 @@
         <v>120</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
@@ -3124,13 +3132,13 @@
         <v>42</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>42</v>
@@ -3148,7 +3156,7 @@
         <v>42</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3166,28 +3174,28 @@
         <v>42</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AN17" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
-    <row r="18" hidden="true">
+    <row r="18">
       <c r="A18" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3197,7 +3205,7 @@
         <v>53</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>42</v>
@@ -3206,17 +3214,17 @@
         <v>54</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>42</v>
@@ -3265,7 +3273,7 @@
         <v>42</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>53</v>
@@ -3280,19 +3288,19 @@
         <v>65</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>42</v>
@@ -3300,7 +3308,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3323,16 +3331,16 @@
         <v>54</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3382,7 +3390,7 @@
         <v>42</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3397,19 +3405,19 @@
         <v>65</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>42</v>
@@ -3417,7 +3425,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3440,16 +3448,16 @@
         <v>54</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3499,7 +3507,7 @@
         <v>42</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3514,19 +3522,19 @@
         <v>65</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>42</v>
@@ -3534,7 +3542,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3557,16 +3565,16 @@
         <v>42</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3616,7 +3624,7 @@
         <v>42</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3625,7 +3633,7 @@
         <v>53</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AI21" t="s" s="2">
         <v>65</v>
@@ -3640,10 +3648,10 @@
         <v>42</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>42</v>
@@ -3651,7 +3659,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3674,13 +3682,13 @@
         <v>54</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3731,7 +3739,7 @@
         <v>42</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -3752,13 +3760,13 @@
         <v>42</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>42</v>
@@ -3766,7 +3774,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3789,13 +3797,13 @@
         <v>54</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -3846,7 +3854,7 @@
         <v>42</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -3870,10 +3878,10 @@
         <v>42</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>42</v>
@@ -3881,7 +3889,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3904,13 +3912,13 @@
         <v>54</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -3961,7 +3969,7 @@
         <v>42</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -3982,13 +3990,13 @@
         <v>42</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>42</v>
@@ -3996,7 +4004,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4019,13 +4027,13 @@
         <v>42</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -4076,7 +4084,7 @@
         <v>42</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4088,7 +4096,7 @@
         <v>42</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>42</v>
@@ -4100,7 +4108,7 @@
         <v>42</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>42</v>
@@ -4111,7 +4119,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4137,10 +4145,10 @@
         <v>55</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4191,7 +4199,7 @@
         <v>42</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4215,7 +4223,7 @@
         <v>42</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>42</v>
@@ -4226,7 +4234,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4255,7 +4263,7 @@
         <v>100</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M27" t="s" s="2">
         <v>102</v>
@@ -4308,7 +4316,7 @@
         <v>42</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4332,7 +4340,7 @@
         <v>42</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>42</v>
@@ -4343,11 +4351,11 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
@@ -4369,10 +4377,10 @@
         <v>99</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M28" t="s" s="2">
         <v>102</v>
@@ -4427,7 +4435,7 @@
         <v>42</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4462,7 +4470,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4488,10 +4496,10 @@
         <v>120</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4518,13 +4526,13 @@
         <v>42</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>42</v>
@@ -4542,7 +4550,7 @@
         <v>42</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4551,7 +4559,7 @@
         <v>53</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>65</v>
@@ -4560,13 +4568,13 @@
         <v>42</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>130</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>42</v>
@@ -4577,7 +4585,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4600,13 +4608,13 @@
         <v>42</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -4657,7 +4665,7 @@
         <v>42</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -4666,7 +4674,7 @@
         <v>44</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>65</v>
@@ -4681,7 +4689,7 @@
         <v>42</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>42</v>
@@ -4692,7 +4700,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4718,10 +4726,10 @@
         <v>120</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -4748,13 +4756,13 @@
         <v>42</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>42</v>
@@ -4772,7 +4780,7 @@
         <v>42</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -4796,7 +4804,7 @@
         <v>42</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>42</v>
@@ -4805,9 +4813,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" hidden="true">
+    <row r="32">
       <c r="A32" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4815,13 +4823,13 @@
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>42</v>
@@ -4830,16 +4838,16 @@
         <v>42</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -4889,7 +4897,7 @@
         <v>42</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -4901,7 +4909,7 @@
         <v>42</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>42</v>
@@ -4913,7 +4921,7 @@
         <v>42</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>42</v>
@@ -4924,7 +4932,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4950,10 +4958,10 @@
         <v>55</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5004,7 +5012,7 @@
         <v>42</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5028,7 +5036,7 @@
         <v>42</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>42</v>
@@ -5039,7 +5047,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5068,7 +5076,7 @@
         <v>100</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>102</v>
@@ -5121,7 +5129,7 @@
         <v>42</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5145,7 +5153,7 @@
         <v>42</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>42</v>
@@ -5156,11 +5164,11 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
@@ -5182,10 +5190,10 @@
         <v>99</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M35" t="s" s="2">
         <v>102</v>
@@ -5240,7 +5248,7 @@
         <v>42</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5275,7 +5283,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5301,10 +5309,10 @@
         <v>120</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5331,13 +5339,13 @@
         <v>42</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>42</v>
@@ -5355,7 +5363,7 @@
         <v>42</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5364,13 +5372,13 @@
         <v>44</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>65</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>150</v>
@@ -5379,10 +5387,10 @@
         <v>42</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>42</v>
@@ -5390,7 +5398,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5398,10 +5406,10 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>42</v>
@@ -5413,13 +5421,13 @@
         <v>54</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5470,7 +5478,7 @@
         <v>42</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5479,7 +5487,7 @@
         <v>44</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>65</v>
@@ -5494,18 +5502,18 @@
         <v>42</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="38" hidden="true">
+    <row r="38">
       <c r="A38" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5516,10 +5524,10 @@
         <v>43</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>42</v>
@@ -5528,13 +5536,13 @@
         <v>42</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5585,7 +5593,7 @@
         <v>42</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5600,16 +5608,16 @@
         <v>65</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>42</v>

</xml_diff>